<commit_message>
allowed tags for toollist
</commit_message>
<xml_diff>
--- a/_data/tool_list.xlsx
+++ b/_data/tool_list.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/353f90cab10cd109/Documenten/Work-DESKTOP-8V2CDT9/rdm-toolkit/_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="61" documentId="8_{191146EF-F505-4547-B871-55E7A17D37A2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{230B800C-8BBC-4144-BA23-E555CAACF42F}"/>
+  <xr:revisionPtr revIDLastSave="63" documentId="8_{191146EF-F505-4547-B871-55E7A17D37A2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{D55139AB-C7FB-4409-930C-800D19359C05}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14595" xr2:uid="{C3B97F62-A39D-4DBC-A677-94D5F0C864A3}"/>
+    <workbookView xWindow="-25320" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{C3B97F62-A39D-4DBC-A677-94D5F0C864A3}"/>
   </bookViews>
   <sheets>
     <sheet name="tools" sheetId="1" r:id="rId1"/>
@@ -566,7 +566,7 @@
   <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>

</xml_diff>

<commit_message>
added phyre as test
</commit_message>
<xml_diff>
--- a/_data/tool_list.xlsx
+++ b/_data/tool_list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/353f90cab10cd109/Documenten/Work-DESKTOP-8V2CDT9/rdm-toolkit/_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="63" documentId="8_{191146EF-F505-4547-B871-55E7A17D37A2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{D55139AB-C7FB-4409-930C-800D19359C05}"/>
+  <xr:revisionPtr revIDLastSave="73" documentId="8_{191146EF-F505-4547-B871-55E7A17D37A2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{5E083D37-D271-40A8-85E9-FC4E999C5B63}"/>
   <bookViews>
     <workbookView xWindow="-25320" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{C3B97F62-A39D-4DBC-A677-94D5F0C864A3}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="57">
   <si>
     <t>link</t>
   </si>
@@ -59,9 +59,6 @@
     <t>Data, model and SOPs management for projects, from preliminary data to publication, support for running SBML models etc.</t>
   </si>
   <si>
-    <t>collect,process, analyse, share, preserve, storage, privacy</t>
-  </si>
-  <si>
     <t>DAISY</t>
   </si>
   <si>
@@ -192,6 +189,24 @@
   </si>
   <si>
     <t>Specification for a standard API for plant data: plant material, plant phenotyping data</t>
+  </si>
+  <si>
+    <t>Phyre2</t>
+  </si>
+  <si>
+    <t>collect, process, analyse, share, preserve, storage, privacy</t>
+  </si>
+  <si>
+    <t>process, analyse</t>
+  </si>
+  <si>
+    <t>http://www.sbg.bio.ic.ac.uk/~phyre2</t>
+  </si>
+  <si>
+    <t>Protein Homology/analogY Recognition Engine</t>
+  </si>
+  <si>
+    <t>phyre</t>
   </si>
 </sst>
 </file>
@@ -563,10 +578,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{607A6159-CF90-4C62-9A5A-46611A956E61}">
-  <dimension ref="A1:E15"/>
+  <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -580,7 +595,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -597,159 +612,159 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>41</v>
-      </c>
       <c r="C2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="C3" t="s">
         <v>37</v>
       </c>
-      <c r="C3" t="s">
+      <c r="E3" t="s">
         <v>38</v>
-      </c>
-      <c r="E3" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="C4" t="s">
         <v>9</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" t="s">
         <v>10</v>
-      </c>
-      <c r="D4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E4" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="C5" t="s">
         <v>34</v>
       </c>
-      <c r="C5" t="s">
-        <v>35</v>
-      </c>
       <c r="E5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="C6" t="s">
         <v>28</v>
       </c>
-      <c r="C6" t="s">
-        <v>29</v>
-      </c>
       <c r="E6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
+        <v>29</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="C7" t="s">
         <v>31</v>
       </c>
-      <c r="C7" t="s">
-        <v>32</v>
-      </c>
       <c r="E7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="C8" t="s">
         <v>22</v>
       </c>
-      <c r="C8" t="s">
-        <v>23</v>
-      </c>
       <c r="E8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="C9" t="s">
         <v>25</v>
       </c>
-      <c r="C9" t="s">
-        <v>26</v>
-      </c>
       <c r="E9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
+        <v>47</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="C10" t="s">
         <v>49</v>
       </c>
-      <c r="C10" t="s">
-        <v>50</v>
-      </c>
       <c r="E10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="C11" t="s">
         <v>18</v>
       </c>
-      <c r="C11" t="s">
+      <c r="E11" t="s">
         <v>19</v>
-      </c>
-      <c r="E11" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
+        <v>44</v>
+      </c>
+      <c r="B12" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="C12" t="s">
         <v>46</v>
       </c>
-      <c r="C12" t="s">
-        <v>47</v>
-      </c>
       <c r="E12" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.45">
@@ -763,32 +778,49 @@
         <v>6</v>
       </c>
       <c r="E13" t="s">
-        <v>7</v>
+        <v>52</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="C14" t="s">
         <v>14</v>
       </c>
-      <c r="C14" t="s">
+      <c r="E14" t="s">
         <v>15</v>
-      </c>
-      <c r="E14" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
+        <v>41</v>
+      </c>
+      <c r="B15" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="C15" t="s">
         <v>43</v>
       </c>
-      <c r="C15" t="s">
-        <v>44</v>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A16" t="s">
+        <v>51</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C16" t="s">
+        <v>55</v>
+      </c>
+      <c r="D16" t="s">
+        <v>56</v>
+      </c>
+      <c r="E16" t="s">
+        <v>53</v>
       </c>
     </row>
   </sheetData>
@@ -812,8 +844,9 @@
     <hyperlink ref="B10" r:id="rId12" xr:uid="{FC038110-0E87-478E-A371-633658B5D905}"/>
     <hyperlink ref="B4" r:id="rId13" xr:uid="{A214AC83-2F44-4B97-8998-E0D885CDAAA6}"/>
     <hyperlink ref="B13" r:id="rId14" xr:uid="{68B02575-576B-4029-A17D-0A39176F2C52}"/>
+    <hyperlink ref="B16" r:id="rId15" xr:uid="{28B18551-5390-49EC-8DCB-A2E3E2C06495}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId15"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId16"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
merge tool list woth resource
</commit_message>
<xml_diff>
--- a/_data/tool_list.xlsx
+++ b/_data/tool_list.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/353f90cab10cd109/Documenten/Work-DESKTOP-8V2CDT9/rdm-toolkit/_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="76" documentId="8_{191146EF-F505-4547-B871-55E7A17D37A2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{4DE93E6D-DB0B-4067-9F04-BF2310360DA3}"/>
+  <xr:revisionPtr revIDLastSave="87" documentId="8_{191146EF-F505-4547-B871-55E7A17D37A2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{B1D0B3FA-636D-46AC-9683-095253E89285}"/>
   <bookViews>
-    <workbookView xWindow="-25320" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{C3B97F62-A39D-4DBC-A677-94D5F0C864A3}"/>
+    <workbookView xWindow="1470" yWindow="1470" windowWidth="16875" windowHeight="10523" xr2:uid="{C3B97F62-A39D-4DBC-A677-94D5F0C864A3}"/>
   </bookViews>
   <sheets>
     <sheet name="tools" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">tools!$A$1:$E$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">tools!$A$1:$F$1</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="71">
   <si>
     <t>link</t>
   </si>
@@ -44,9 +44,6 @@
     <t>description</t>
   </si>
   <si>
-    <t>biotoolsid</t>
-  </si>
-  <si>
     <t>tags</t>
   </si>
   <si>
@@ -207,6 +204,51 @@
   </si>
   <si>
     <t>phyre</t>
+  </si>
+  <si>
+    <t>MIAPPE</t>
+  </si>
+  <si>
+    <t>https://www.miappe.org/</t>
+  </si>
+  <si>
+    <t>Minimum Information About a Plant Phenotyping Experiment</t>
+  </si>
+  <si>
+    <t>nd9ce9</t>
+  </si>
+  <si>
+    <t>standard</t>
+  </si>
+  <si>
+    <t>maDMP - Research Bridge</t>
+  </si>
+  <si>
+    <t>https://library.ust.hk/sc/machine-actionable-dmp/</t>
+  </si>
+  <si>
+    <t>Machine-Actionable Data Management Plan | Webinar (2016) on making a good data management plan</t>
+  </si>
+  <si>
+    <t>Research Management Plan</t>
+  </si>
+  <si>
+    <t>https://researcheracademy.elsevier.com/research-preparation/research-data-management/creating-good-research-data-management-plan</t>
+  </si>
+  <si>
+    <t>Machine actionable DMPs</t>
+  </si>
+  <si>
+    <t>tool</t>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>resource</t>
+  </si>
+  <si>
+    <t>registry</t>
   </si>
 </sst>
 </file>
@@ -578,10 +620,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{607A6159-CF90-4C62-9A5A-46611A956E61}">
-  <dimension ref="A1:E16"/>
+  <dimension ref="A1:F19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -589,13 +631,14 @@
     <col min="1" max="1" width="16.86328125" customWidth="1"/>
     <col min="2" max="2" width="19.19921875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="100.06640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.86328125" customWidth="1"/>
-    <col min="5" max="5" width="45.796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.3984375" customWidth="1"/>
+    <col min="5" max="5" width="16.86328125" customWidth="1"/>
+    <col min="6" max="6" width="45.796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -604,228 +647,330 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D2" t="s">
+        <v>67</v>
+      </c>
+      <c r="F2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D3" t="s">
+        <v>67</v>
+      </c>
+      <c r="F3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" t="s">
+        <v>67</v>
+      </c>
+      <c r="E4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D5" t="s">
+        <v>67</v>
+      </c>
+      <c r="F5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C6" t="s">
+        <v>27</v>
+      </c>
+      <c r="D6" t="s">
+        <v>67</v>
+      </c>
+      <c r="F6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A7" t="s">
+        <v>28</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C7" t="s">
+        <v>30</v>
+      </c>
+      <c r="D7" t="s">
+        <v>67</v>
+      </c>
+      <c r="F7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" t="s">
+        <v>21</v>
+      </c>
+      <c r="D8" t="s">
+        <v>67</v>
+      </c>
+      <c r="F8" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A9" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" t="s">
+        <v>24</v>
+      </c>
+      <c r="D9" t="s">
+        <v>67</v>
+      </c>
+      <c r="F9" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A10" t="s">
+        <v>46</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C10" t="s">
+        <v>48</v>
+      </c>
+      <c r="D10" t="s">
+        <v>67</v>
+      </c>
+      <c r="F10" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A11" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C11" t="s">
+        <v>17</v>
+      </c>
+      <c r="D11" t="s">
+        <v>67</v>
+      </c>
+      <c r="F11" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A12" t="s">
+        <v>43</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C12" t="s">
+        <v>45</v>
+      </c>
+      <c r="D12" t="s">
+        <v>67</v>
+      </c>
+      <c r="F12" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A13" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A2" t="s">
-        <v>39</v>
-      </c>
-      <c r="B2" s="2" t="s">
+      <c r="B13" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C13" t="s">
+        <v>5</v>
+      </c>
+      <c r="D13" t="s">
+        <v>67</v>
+      </c>
+      <c r="F13" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A14" t="s">
+        <v>11</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C14" t="s">
+        <v>13</v>
+      </c>
+      <c r="D14" t="s">
+        <v>67</v>
+      </c>
+      <c r="F14" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A15" t="s">
         <v>40</v>
       </c>
-      <c r="C2" t="s">
+      <c r="B15" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C15" t="s">
+        <v>42</v>
+      </c>
+      <c r="D15" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A16" t="s">
         <v>50</v>
       </c>
-      <c r="E2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A3" t="s">
-        <v>35</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="C3" t="s">
-        <v>37</v>
-      </c>
-      <c r="E3" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A5" t="s">
-        <v>32</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="C5" t="s">
-        <v>34</v>
-      </c>
-      <c r="E5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A6" t="s">
-        <v>26</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C6" t="s">
-        <v>28</v>
-      </c>
-      <c r="E6" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A7" t="s">
-        <v>29</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="C7" t="s">
-        <v>31</v>
-      </c>
-      <c r="E7" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A8" t="s">
-        <v>20</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C8" t="s">
-        <v>22</v>
-      </c>
-      <c r="E8" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A9" t="s">
-        <v>23</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C9" t="s">
-        <v>25</v>
-      </c>
-      <c r="E9" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A10" t="s">
-        <v>47</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="C10" t="s">
-        <v>49</v>
-      </c>
-      <c r="E10" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A11" t="s">
-        <v>16</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C11" t="s">
+      <c r="B16" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C16" t="s">
+        <v>54</v>
+      </c>
+      <c r="D16" t="s">
+        <v>67</v>
+      </c>
+      <c r="E16" t="s">
+        <v>55</v>
+      </c>
+      <c r="F16" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A17" t="s">
+        <v>56</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C17" t="s">
+        <v>58</v>
+      </c>
+      <c r="D17" t="s">
+        <v>69</v>
+      </c>
+      <c r="E17" t="s">
+        <v>59</v>
+      </c>
+      <c r="F17" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A18" t="s">
+        <v>61</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C18" t="s">
+        <v>63</v>
+      </c>
+      <c r="D18" t="s">
+        <v>69</v>
+      </c>
+      <c r="F18" t="s">
         <v>18</v>
       </c>
-      <c r="E11" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A12" t="s">
-        <v>44</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="C12" t="s">
-        <v>46</v>
-      </c>
-      <c r="E12" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A13" t="s">
-        <v>4</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C13" t="s">
-        <v>6</v>
-      </c>
-      <c r="E13" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A14" t="s">
-        <v>12</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C14" t="s">
-        <v>14</v>
-      </c>
-      <c r="E14" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A15" t="s">
-        <v>41</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="C15" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A16" t="s">
-        <v>51</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="C16" t="s">
-        <v>55</v>
-      </c>
-      <c r="D16" t="s">
-        <v>56</v>
-      </c>
-      <c r="E16" t="s">
-        <v>53</v>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A19" t="s">
+        <v>64</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="C19" t="s">
+        <v>66</v>
+      </c>
+      <c r="D19" t="s">
+        <v>69</v>
+      </c>
+      <c r="F19" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E1" xr:uid="{DF25C546-BE4B-446A-96BF-056CCF94994B}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E15">
+  <autoFilter ref="A1:F1" xr:uid="{DF25C546-BE4B-446A-96BF-056CCF94994B}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F15">
       <sortCondition ref="A1"/>
     </sortState>
   </autoFilter>
@@ -845,8 +990,11 @@
     <hyperlink ref="B13" r:id="rId13" xr:uid="{68B02575-576B-4029-A17D-0A39176F2C52}"/>
     <hyperlink ref="B16" r:id="rId14" xr:uid="{28B18551-5390-49EC-8DCB-A2E3E2C06495}"/>
     <hyperlink ref="B2" r:id="rId15" xr:uid="{4B56C4F7-A988-4A02-AEB0-E6FB3032D08C}"/>
+    <hyperlink ref="B17" r:id="rId16" xr:uid="{9F98CF53-0B72-47BE-8D04-1077A58AF019}"/>
+    <hyperlink ref="B18" r:id="rId17" xr:uid="{5C086763-FD38-40EF-8258-B094B2C54FFD}"/>
+    <hyperlink ref="B19" r:id="rId18" xr:uid="{CF171061-8B97-4631-B557-47D919636E1A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId16"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId19"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
different handling of registries
</commit_message>
<xml_diff>
--- a/_data/tool_list.xlsx
+++ b/_data/tool_list.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/353f90cab10cd109/Documenten/Work-DESKTOP-8V2CDT9/rdm-toolkit/_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="89" documentId="8_{191146EF-F505-4547-B871-55E7A17D37A2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{62A0FF95-A009-43DB-B4C6-B4B6EEF024F8}"/>
+  <xr:revisionPtr revIDLastSave="98" documentId="8_{191146EF-F505-4547-B871-55E7A17D37A2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{56EFE235-61A5-4673-842B-B073C1E4FE6D}"/>
   <bookViews>
-    <workbookView xWindow="1470" yWindow="1470" windowWidth="16875" windowHeight="10523" xr2:uid="{C3B97F62-A39D-4DBC-A677-94D5F0C864A3}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14595" xr2:uid="{C3B97F62-A39D-4DBC-A677-94D5F0C864A3}"/>
   </bookViews>
   <sheets>
     <sheet name="tools" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">tools!$A$1:$F$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">tools!$A$1:$E$1</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="69">
   <si>
     <t>link</t>
   </si>
@@ -203,9 +203,6 @@
     <t>Protein Homology/analogY Recognition Engine</t>
   </si>
   <si>
-    <t>phyre</t>
-  </si>
-  <si>
     <t>MIAPPE</t>
   </si>
   <si>
@@ -215,9 +212,6 @@
     <t>Minimum Information About a Plant Phenotyping Experiment</t>
   </si>
   <si>
-    <t>nd9ce9</t>
-  </si>
-  <si>
     <t>standard</t>
   </si>
   <si>
@@ -239,16 +233,16 @@
     <t>Machine actionable DMPs</t>
   </si>
   <si>
-    <t>tool</t>
-  </si>
-  <si>
-    <t>type</t>
-  </si>
-  <si>
-    <t>resource</t>
-  </si>
-  <si>
     <t>registry</t>
+  </si>
+  <si>
+    <t>biotools:DAISY</t>
+  </si>
+  <si>
+    <t>biotools:phyre</t>
+  </si>
+  <si>
+    <t>fairsharing:nd9ce9</t>
   </si>
 </sst>
 </file>
@@ -620,10 +614,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{607A6159-CF90-4C62-9A5A-46611A956E61}">
-  <dimension ref="A1:F19"/>
+  <dimension ref="A1:E19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -631,12 +625,11 @@
     <col min="1" max="1" width="16.86328125" customWidth="1"/>
     <col min="2" max="2" width="19.19921875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="100.06640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.3984375" customWidth="1"/>
-    <col min="5" max="5" width="16.86328125" customWidth="1"/>
-    <col min="6" max="6" width="45.796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.86328125" customWidth="1"/>
+    <col min="5" max="5" width="45.796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>10</v>
       </c>
@@ -647,16 +640,13 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="F1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>38</v>
       </c>
@@ -666,14 +656,11 @@
       <c r="C2" t="s">
         <v>49</v>
       </c>
-      <c r="D2" t="s">
-        <v>67</v>
-      </c>
-      <c r="F2" t="s">
+      <c r="E2" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>34</v>
       </c>
@@ -683,14 +670,11 @@
       <c r="C3" t="s">
         <v>36</v>
       </c>
-      <c r="D3" t="s">
-        <v>67</v>
-      </c>
-      <c r="F3" t="s">
+      <c r="E3" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -701,16 +685,13 @@
         <v>8</v>
       </c>
       <c r="D4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E4" t="s">
-        <v>6</v>
-      </c>
-      <c r="F4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>31</v>
       </c>
@@ -720,14 +701,11 @@
       <c r="C5" t="s">
         <v>33</v>
       </c>
-      <c r="D5" t="s">
-        <v>67</v>
-      </c>
-      <c r="F5" t="s">
+      <c r="E5" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>25</v>
       </c>
@@ -737,14 +715,11 @@
       <c r="C6" t="s">
         <v>27</v>
       </c>
-      <c r="D6" t="s">
-        <v>67</v>
-      </c>
-      <c r="F6" t="s">
+      <c r="E6" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>28</v>
       </c>
@@ -754,14 +729,11 @@
       <c r="C7" t="s">
         <v>30</v>
       </c>
-      <c r="D7" t="s">
-        <v>67</v>
-      </c>
-      <c r="F7" t="s">
+      <c r="E7" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>19</v>
       </c>
@@ -771,14 +743,11 @@
       <c r="C8" t="s">
         <v>21</v>
       </c>
-      <c r="D8" t="s">
-        <v>67</v>
-      </c>
-      <c r="F8" t="s">
+      <c r="E8" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>22</v>
       </c>
@@ -788,14 +757,11 @@
       <c r="C9" t="s">
         <v>24</v>
       </c>
-      <c r="D9" t="s">
-        <v>67</v>
-      </c>
-      <c r="F9" t="s">
+      <c r="E9" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>46</v>
       </c>
@@ -805,14 +771,11 @@
       <c r="C10" t="s">
         <v>48</v>
       </c>
-      <c r="D10" t="s">
-        <v>67</v>
-      </c>
-      <c r="F10" t="s">
+      <c r="E10" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>15</v>
       </c>
@@ -822,14 +785,11 @@
       <c r="C11" t="s">
         <v>17</v>
       </c>
-      <c r="D11" t="s">
-        <v>67</v>
-      </c>
-      <c r="F11" t="s">
+      <c r="E11" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>43</v>
       </c>
@@ -839,14 +799,11 @@
       <c r="C12" t="s">
         <v>45</v>
       </c>
-      <c r="D12" t="s">
-        <v>67</v>
-      </c>
-      <c r="F12" t="s">
+      <c r="E12" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>3</v>
       </c>
@@ -856,14 +813,11 @@
       <c r="C13" t="s">
         <v>5</v>
       </c>
-      <c r="D13" t="s">
-        <v>67</v>
-      </c>
-      <c r="F13" t="s">
+      <c r="E13" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>11</v>
       </c>
@@ -873,14 +827,11 @@
       <c r="C14" t="s">
         <v>13</v>
       </c>
-      <c r="D14" t="s">
-        <v>67</v>
-      </c>
-      <c r="F14" t="s">
+      <c r="E14" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>40</v>
       </c>
@@ -890,11 +841,8 @@
       <c r="C15" t="s">
         <v>42</v>
       </c>
-      <c r="D15" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>50</v>
       </c>
@@ -908,69 +856,57 @@
         <v>67</v>
       </c>
       <c r="E16" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A17" t="s">
         <v>55</v>
       </c>
-      <c r="F16" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A17" t="s">
+      <c r="B17" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="C17" t="s">
         <v>57</v>
       </c>
-      <c r="C17" t="s">
+      <c r="D17" t="s">
+        <v>68</v>
+      </c>
+      <c r="E17" t="s">
         <v>58</v>
       </c>
-      <c r="D17" t="s">
-        <v>69</v>
-      </c>
-      <c r="E17" t="s">
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A18" t="s">
         <v>59</v>
       </c>
-      <c r="F17" t="s">
+      <c r="B18" s="2" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A18" t="s">
+      <c r="C18" t="s">
         <v>61</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="E18" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A19" t="s">
         <v>62</v>
       </c>
-      <c r="C18" t="s">
+      <c r="B19" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="D18" t="s">
-        <v>69</v>
-      </c>
-      <c r="F18" t="s">
+      <c r="C19" t="s">
+        <v>64</v>
+      </c>
+      <c r="E19" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A19" t="s">
-        <v>64</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="C19" t="s">
-        <v>66</v>
-      </c>
-      <c r="D19" t="s">
-        <v>69</v>
-      </c>
-      <c r="F19" t="s">
-        <v>18</v>
-      </c>
-    </row>
   </sheetData>
-  <autoFilter ref="A1:F1" xr:uid="{DF25C546-BE4B-446A-96BF-056CCF94994B}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F15">
+  <autoFilter ref="A1:E1" xr:uid="{DF25C546-BE4B-446A-96BF-056CCF94994B}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E15">
       <sortCondition ref="A1"/>
     </sortState>
   </autoFilter>

</xml_diff>